<commit_message>
Added code to access the value of a specific dimension of a core from the spreadsheet
</commit_message>
<xml_diff>
--- a/PandasSubtablePractice.xlsx
+++ b/PandasSubtablePractice.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19725\Desktop\education\college\extracurriculars\pemg research\random python scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19725\Desktop\education\college\extracurriculars\pemg research\PEMG_Design_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DB40B7-CD12-422A-9872-0A1DBAB150BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE779FF1-D552-499C-B774-7C3D0CDBC70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -451,6 +451,7 @@
         <v>1</v>
       </c>
     </row>
+    <row r="12" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>